<commit_message>
Create single sticker is working
</commit_message>
<xml_diff>
--- a/src/graphics-design/sticker/Stiker Meassures.xlsx
+++ b/src/graphics-design/sticker/Stiker Meassures.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinir\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\personal-git\aresta-barcode\src\graphics-design\sticker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D1BACDB-8783-4A0D-A1D1-B16C8CA9B25C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4470FF71-E0CF-44A4-918A-9A8EC3AEDA73}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4005" yWindow="2310" windowWidth="21600" windowHeight="11385" xr2:uid="{8C9913A1-B810-4F19-872C-43348DC68D8C}"/>
+    <workbookView xWindow="11160" yWindow="1830" windowWidth="6645" windowHeight="11970" xr2:uid="{8C9913A1-B810-4F19-872C-43348DC68D8C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Stiker</t>
   </si>
@@ -55,6 +55,21 @@
   </si>
   <si>
     <t>Header APT each number</t>
+  </si>
+  <si>
+    <t>header</t>
+  </si>
+  <si>
+    <t>digit1</t>
+  </si>
+  <si>
+    <t>digit2</t>
+  </si>
+  <si>
+    <t>Pad</t>
+  </si>
+  <si>
+    <t>Padding</t>
   </si>
 </sst>
 </file>
@@ -96,7 +111,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -406,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09B54DC7-1CC7-43F4-9C21-6E9EF61AE171}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -492,7 +518,73 @@
         <v>114</v>
       </c>
     </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>68</v>
+      </c>
+      <c r="C11">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>584</v>
+      </c>
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f>SUM(B21:D21)</f>
+        <v>584</v>
+      </c>
+      <c r="B21">
+        <v>420</v>
+      </c>
+      <c r="C21">
+        <v>82</v>
+      </c>
+      <c r="D21">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f>SUM(B22:E22)</f>
+        <v>584</v>
+      </c>
+      <c r="B22">
+        <v>420</v>
+      </c>
+      <c r="C22">
+        <v>48</v>
+      </c>
+      <c r="D22">
+        <v>48</v>
+      </c>
+      <c r="E22">
+        <v>68</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="A20:A22">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>584</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>